<commit_message>
first model for the path following controller
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Master\Path Planning and Controll\Projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89242F6C-F878-4BEE-86F4-C53D9900FC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40A3A9E-C143-45B2-BB5B-FEBD97959660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42705" yWindow="2070" windowWidth="19200" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Guidelines</t>
   </si>
@@ -582,13 +583,25 @@
   </si>
   <si>
     <t>s6_data.m aufrufen, wenn Simulink Model startet über Init() - Funktion</t>
+  </si>
+  <si>
+    <t>ToDos</t>
+  </si>
+  <si>
+    <t>Code aus Aufgabe in Bericht oder in Ordner lassen?</t>
+  </si>
+  <si>
+    <t>Aufgabe</t>
+  </si>
+  <si>
+    <t>8.3.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +633,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -641,11 +662,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,7 +683,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -959,81 +981,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.90625" customWidth="1"/>
+    <col min="1" max="1" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1042,4 +1064,35 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E991BC7E-4FD8-4CF2-A7D9-67B21F4E95E6}">
+  <dimension ref="B2:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
viele FUnktionen dokumentiert; Verbindungen verbessert, weniger Kreuzungen; beim Switch Speed Controller haben wir jetzt eine MatLab Function
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40A3A9E-C143-45B2-BB5B-FEBD97959660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0F64F3-7C37-4AE6-8D85-C2C475FD342F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Guidelines</t>
   </si>
@@ -313,6 +313,268 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Variable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mit einem</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> P_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> um </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parameter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> von </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Signalen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zu spesfizieren </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pyhsikalisch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>größe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> müssen angegeben werden durch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Block annotations</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parameter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> als </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Workspace variabel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> definieren sowie </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kommentare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mit der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Einheit</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabenstellungen am ende jedes Kapitels sollen rausgeschrieben werden </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ergebnisse kurz dokumentieren </t>
+  </si>
+  <si>
+    <t>s6_data.m aufrufen, wenn Simulink Model startet über Init() - Funktion</t>
+  </si>
+  <si>
+    <t>ToDos</t>
+  </si>
+  <si>
+    <t>Code aus Aufgabe in Bericht oder in Ordner lassen?</t>
+  </si>
+  <si>
+    <t>Aufgabe</t>
+  </si>
+  <si>
+    <t>8.3.2</t>
+  </si>
+  <si>
+    <t>Lösung</t>
+  </si>
+  <si>
+    <t>nicht in Bericht aber auf entsprechendes File verweisen</t>
+  </si>
+  <si>
+    <t>Fertig</t>
+  </si>
+  <si>
+    <t>Nur Subsysteme oder Modellreferenzen auf oberstem Modell Level (keine anderen Blöcke)</t>
+  </si>
+  <si>
+    <t>Subsysteme oder allgemeine Modelle sollen nicht mehr als 7 Blöcke haben</t>
+  </si>
+  <si>
+    <t>keine Umlaute oder spezielle Character verwenden</t>
+  </si>
+  <si>
+    <t>Numerisch: alle Solver sollen mit Fixed-Step P_dt arbeiten</t>
+  </si>
+  <si>
+    <t>nur elementare Blöcke verwenden, nichts komplexes wie diskrete oder kontinuierliche Transfer Functions oder PID Controller vom Simulink Blockset</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Signale</t>
     </r>
     <r>
@@ -357,244 +619,25 @@
       </rPr>
       <t>Namen</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Variable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> mit einem</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> P_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> um </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Parameter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> von </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Signalen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> zu spesfizieren </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pyhsikalisch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>größe</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> müssen angegeben werden durch </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Block annotations</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Parameter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> als </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Workspace variabel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> definieren sowie </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>kommentare</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> mit der </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Einheit</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufgabenstellungen am ende jedes Kapitels sollen rausgeschrieben werden </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ergebnisse kurz dokumentieren </t>
-  </si>
-  <si>
-    <t>s6_data.m aufrufen, wenn Simulink Model startet über Init() - Funktion</t>
-  </si>
-  <si>
-    <t>ToDos</t>
-  </si>
-  <si>
-    <t>Code aus Aufgabe in Bericht oder in Ordner lassen?</t>
-  </si>
-  <si>
-    <t>Aufgabe</t>
-  </si>
-  <si>
-    <t>8.3.2</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> entsprechend C-Konvention</t>
+    </r>
+  </si>
+  <si>
+    <t>Alles Englisch</t>
+  </si>
+  <si>
+    <t>MatLab Funktionen Dokumentieren oben</t>
+  </si>
+  <si>
+    <t>Alle Systeme fertig bis auf die low-level von Vehicle Dynamics</t>
   </si>
 </sst>
 </file>
@@ -662,9 +705,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,74 +1037,126 @@
     <col min="1" max="1" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1068,28 +1167,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E991BC7E-4FD8-4CF2-A7D9-67B21F4E95E6}">
-  <dimension ref="B2:H4"/>
+  <dimension ref="B2:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weiter aufgeräumt in Vehicle Dynamics: mehr MatLab Functions anstatt vieler einzelner Subsysteme --> jetzt weniger Verbindungen, die sich kreuzen
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0F64F3-7C37-4AE6-8D85-C2C475FD342F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1164F8-4BAE-43B0-930B-E60FA74076D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Guidelines</t>
   </si>
@@ -638,13 +638,22 @@
   </si>
   <si>
     <t>Alle Systeme fertig bis auf die low-level von Vehicle Dynamics</t>
+  </si>
+  <si>
+    <t>Mehr Matlab Funktionen?</t>
+  </si>
+  <si>
+    <t>manche mehr</t>
+  </si>
+  <si>
+    <t>Diskrete  Übtgsfkt. In Position Controller Guvp1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,13 +693,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -705,13 +739,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,138 +1064,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.85546875" customWidth="1"/>
+    <col min="1" max="1" width="72.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
+      <c r="B22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
code clean in bezug auf Vehical Dynamic-> LowSpeed and High Speed Controller
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Master\Path Planning and Controll\Projekt\Part_1\matlab\madctrl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1164F8-4BAE-43B0-930B-E60FA74076D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2C4615-4C3F-4E31-A9FF-499DBB773BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Guidelines</t>
   </si>
@@ -637,9 +637,6 @@
     <t>MatLab Funktionen Dokumentieren oben</t>
   </si>
   <si>
-    <t>Alle Systeme fertig bis auf die low-level von Vehicle Dynamics</t>
-  </si>
-  <si>
     <t>Mehr Matlab Funktionen?</t>
   </si>
   <si>
@@ -647,6 +644,18 @@
   </si>
   <si>
     <t>Diskrete  Übtgsfkt. In Position Controller Guvp1</t>
+  </si>
+  <si>
+    <t>Abnahme Aaron</t>
+  </si>
+  <si>
+    <t>Abnahme Heiko</t>
+  </si>
+  <si>
+    <t>Finale Controlle</t>
+  </si>
+  <si>
+    <t>Speedcontroller???</t>
   </si>
 </sst>
 </file>
@@ -727,7 +736,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -735,11 +744,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -750,9 +821,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -768,7 +846,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1064,156 +1142,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="72.42578125" customWidth="1"/>
+    <col min="1" max="1" width="72.453125" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>45286</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>45286</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>45286</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4"/>
       <c r="D15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="7"/>
       <c r="D18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="6"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1229,9 +1365,9 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1242,7 +1378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Path Controller almost working; Spline import misses the "periodic" property
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1164F8-4BAE-43B0-930B-E60FA74076D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAB76A4-DB54-4498-8065-A5D4BDD86A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -1195,7 +1195,7 @@
       <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">

</xml_diff>

<commit_message>
added lab documentation until Bahnfolgeregelung
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01EEEB4-8A02-45BA-8EEA-FA9D260629F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8490E76F-CEF7-4E81-8E0B-A57BEBA36486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -810,10 +810,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1145,299 +1144,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="B3" s="5"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>45286</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
+      <c r="B5" s="4"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
+      <c r="B6" s="5"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>45286</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>45286</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13"/>
+      <c r="B11" s="7"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13"/>
+      <c r="B12" s="7"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="13"/>
+      <c r="B13" s="5"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="5"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="7"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="6"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="B18" s="7"/>
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
+      <c r="B19" s="6"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
+      <c r="B20" s="5"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="B22" s="4"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1447,15 +1359,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E991BC7E-4FD8-4CF2-A7D9-67B21F4E95E6}">
-  <dimension ref="B2:J4"/>
+  <dimension ref="B2:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1466,16 +1378,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
die inputs outputs sind wieder alle farbig sowie die Funktionsbeschreibungen der Vorsteuerung und Zustandsregler
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Master\Path Planning and Controll\Projekt\Part_1\matlab\madctrl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2FF536-C3FB-42A2-9C0C-79691C22F40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAFA92C-065D-4183-9FCC-2418E7445BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Guidelines</t>
   </si>
@@ -659,6 +659,9 @@
   </si>
   <si>
     <t>Position Controller: G_vp1 --&gt; P_p_T oder P_p_TA für Hochpass Filter?</t>
+  </si>
+  <si>
+    <t>Müssen konst blöcke auch?</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -849,7 +852,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1147,11 +1150,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
@@ -1190,7 +1193,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="8">
-        <v>45286</v>
+        <v>45293</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="12"/>
@@ -1237,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8">
-        <v>45286</v>
+        <v>45293</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
@@ -1247,7 +1250,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="8">
-        <v>45286</v>
+        <v>45293</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="12"/>
@@ -1364,11 +1370,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E991BC7E-4FD8-4CF2-A7D9-67B21F4E95E6}">
   <dimension ref="B2:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
function documentation improved, small changes
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\Master\Path Planning and Controll\Projekt\Part_1\matlab\madctrl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAFA92C-065D-4183-9FCC-2418E7445BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A929A03-F4FA-4B12-A6D7-82E984CCC609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Guidelines</t>
   </si>
@@ -662,6 +662,9 @@
   </si>
   <si>
     <t>Müssen konst blöcke auch?</t>
+  </si>
+  <si>
+    <t>ist global eingestellt</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -834,9 +837,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -852,7 +856,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1151,10 +1155,10 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
@@ -1202,7 +1206,7 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="15"/>
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
     </row>
@@ -1305,7 +1309,7 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="5"/>
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
     </row>
@@ -1313,7 +1317,10 @@
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="12"/>
     </row>
@@ -1374,7 +1381,7 @@
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
updated doc and excel
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\OneDrive - bwedu\Mechatronik und Robotik\Semester 2\AS Path Planning and Control\Projekt\HS_Path_Planning_and_Control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studhsheilbronnde-my.sharepoint.com/personal/akiani_stud_hs-heilbronn_de/Documents/Mechatronik und Robotik/Semester 2/AS Path Planning and Control/Projekt/HS_Path_Planning_and_Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A929A03-F4FA-4B12-A6D7-82E984CCC609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{3A929A03-F4FA-4B12-A6D7-82E984CCC609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D19AB29-31E4-4CBF-AD5A-221D45486152}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2130" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Guidelines</t>
   </si>
@@ -665,13 +665,68 @@
   </si>
   <si>
     <t>ist global eingestellt</t>
+  </si>
+  <si>
+    <t>Signal-Zeit-Diagramme von Sprungantworten der Fahrzeuggeschwindigkeit v_r aus Simulink-MiL-Simulationen und auf dem realen MAD-System</t>
+  </si>
+  <si>
+    <t>S.205</t>
+  </si>
+  <si>
+    <t>Wert und Einheit von k_p</t>
+  </si>
+  <si>
+    <t>S.223</t>
+  </si>
+  <si>
+    <t>welche Einheit?</t>
+  </si>
+  <si>
+    <t>S.224</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Signal-Zeit-Diagramme der Sollposition </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="CambriaMath"/>
+      </rPr>
+      <t xml:space="preserve">𝑤p(𝑡) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="DGMetaSerifScience-Regular"/>
+      </rPr>
+      <t xml:space="preserve">und der Istposition </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="CambriaMath"/>
+      </rPr>
+      <t>yp(𝑡) = x(𝑡)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="DGMetaSerifScience-Regular"/>
+      </rPr>
+      <t xml:space="preserve"> aus Simulink-MiL-Simulationen und auf dem realen MAD-System</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -717,6 +772,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="DGMetaSerifScience-Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="CambriaMath"/>
     </font>
   </fonts>
   <fills count="5">
@@ -819,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -838,9 +903,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -856,7 +922,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1154,18 +1220,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="72.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,7 +1239,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1184,7 +1250,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1192,7 +1258,7 @@
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1202,7 +1268,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1276,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1218,7 +1284,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1295,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1305,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1249,7 +1315,7 @@
       <c r="G9" s="11"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1328,7 @@
       <c r="G10" s="11"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1270,7 +1336,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1278,7 +1344,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1286,7 +1352,7 @@
       <c r="G13" s="11"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1294,7 +1360,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1305,7 +1371,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1313,7 +1379,7 @@
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1324,7 +1390,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1401,7 @@
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1343,7 +1409,7 @@
       <c r="G19" s="11"/>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1351,7 +1417,7 @@
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1359,7 +1425,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1375,15 +1441,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E991BC7E-4FD8-4CF2-A7D9-67B21F4E95E6}">
-  <dimension ref="B2:O5"/>
+  <dimension ref="B2:Q11"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" ht="18.75">
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1394,7 +1460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1416,7 +1482,7 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17">
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1429,6 +1495,36 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>